<commit_message>
Added Couple of more requirments
</commit_message>
<xml_diff>
--- a/functional_requirements_rough_ideas.xlsx
+++ b/functional_requirements_rough_ideas.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuconestogacon-my.sharepoint.com/personal/dbolanososejo6481_conestogac_on_ca/Documents/Big Data Solutions Architecture/Programmig for Big Data/Big-Data-Project-Group-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Second Course\Programming in Big Data\Project\Big-Data-Project-Group-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{37B535D4-57E4-CE4A-9F7C-E36D3FE9CDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DDA7CF0-0C73-BA42-B026-7D74E4C4322D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D56F8-27D6-4D05-8C72-C2659E7BE2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="4" xr2:uid="{1E7BD504-4860-486C-9451-4D7E4421BCCA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="11" xr2:uid="{1E7BD504-4860-486C-9451-4D7E4421BCCA}"/>
   </bookViews>
   <sheets>
     <sheet name="User management" sheetId="3" r:id="rId1"/>
     <sheet name="Grocery" sheetId="4" r:id="rId2"/>
-    <sheet name="Price Comparison" sheetId="5" r:id="rId3"/>
-    <sheet name="Search" sheetId="6" r:id="rId4"/>
-    <sheet name="Notification" sheetId="7" r:id="rId5"/>
-    <sheet name="In Store Navigation" sheetId="8" r:id="rId6"/>
-    <sheet name="Inventory" sheetId="9" r:id="rId7"/>
-    <sheet name="Cart" sheetId="10" r:id="rId8"/>
-    <sheet name="Reporting" sheetId="11" r:id="rId9"/>
-    <sheet name="Review" sheetId="12" r:id="rId10"/>
-    <sheet name="system" sheetId="13" r:id="rId11"/>
+    <sheet name="Favourite Store" sheetId="15" r:id="rId3"/>
+    <sheet name="Price Comparison" sheetId="5" r:id="rId4"/>
+    <sheet name="Search" sheetId="6" r:id="rId5"/>
+    <sheet name="Notification" sheetId="7" r:id="rId6"/>
+    <sheet name="In Store Navigation" sheetId="8" r:id="rId7"/>
+    <sheet name="Inventory" sheetId="9" r:id="rId8"/>
+    <sheet name="Cart" sheetId="10" r:id="rId9"/>
+    <sheet name="Reporting" sheetId="11" r:id="rId10"/>
+    <sheet name="Review" sheetId="12" r:id="rId11"/>
+    <sheet name="system" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Functional Requirement</t>
   </si>
@@ -238,6 +239,69 @@
   </si>
   <si>
     <t>Cart products remains on cache for easy pick up for next time</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>System will display the product limit of the items (if specified)</t>
+  </si>
+  <si>
+    <t>User can search for an items by grocery store name</t>
+  </si>
+  <si>
+    <t>e.g Lime in Walmart</t>
+  </si>
+  <si>
+    <t>User can search for the entire flyer of a particular grocery store</t>
+  </si>
+  <si>
+    <t>e.g Walmart</t>
+  </si>
+  <si>
+    <t>System will display the offered price validity</t>
+  </si>
+  <si>
+    <t>User will receive notifications regarding price drops or offer regaring the recent item searched by the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can add or change colours of aisles </t>
+  </si>
+  <si>
+    <t>If its an organic aisle, admin can add light green colour to it</t>
+  </si>
+  <si>
+    <t>Admin can add or change aisles names or item category</t>
+  </si>
+  <si>
+    <t>User can mark their favourite grocery store</t>
+  </si>
+  <si>
+    <t>Admin can add or update grocery stores they price match with</t>
+  </si>
+  <si>
+    <t>Admin can add or update the quantity of items they can price match</t>
+  </si>
+  <si>
+    <t>Product quantity</t>
+  </si>
+  <si>
+    <t>User can see some most trending searches of current week, searched by other user</t>
+  </si>
+  <si>
+    <t>User will get notification when new flyer launches every week of their favourite grocery store.</t>
+  </si>
+  <si>
+    <t>User can search for an item in the store and, it will give them the aisle number for the item</t>
+  </si>
+  <si>
+    <t>Allows user to check their total cart amount  once they add items in the cart</t>
+  </si>
+  <si>
+    <t>It benefits the user to carry necessary cash.</t>
+  </si>
+  <si>
+    <t>User can update the item quantity (default 1)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -506,11 +570,177 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1005,38 +1235,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7ABED239-953B-4D1A-AAED-2CA50DC64A79}" name="Table2" displayName="Table2" ref="A1:D33" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7ABED239-953B-4D1A-AAED-2CA50DC64A79}" name="Table2" displayName="Table2" ref="A1:D33" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A9AAF479-6EAE-4B0A-992D-CA207A29F62D}" name="Functional Requirement" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{7B0437CB-36EA-49A4-A4D4-DF916F9DC1E4}" name="Notes" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{C95A1AD0-C500-4607-9584-B943104F1CFC}" name="Priority" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{7CE6D686-41F8-4548-8D9C-F62C73745A22}" name="Proposed By" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{A9AAF479-6EAE-4B0A-992D-CA207A29F62D}" name="Functional Requirement" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{7B0437CB-36EA-49A4-A4D4-DF916F9DC1E4}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{C95A1AD0-C500-4607-9584-B943104F1CFC}" name="Priority" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{7CE6D686-41F8-4548-8D9C-F62C73745A22}" name="Proposed By" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E3953504-9D1B-481C-AD87-36BE767B8EC0}" name="Table24" displayName="Table24" ref="A1:D33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E3953504-9D1B-481C-AD87-36BE767B8EC0}" name="Table24" displayName="Table24" ref="A1:D33" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:D33" xr:uid="{E3953504-9D1B-481C-AD87-36BE767B8EC0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CFF24DCB-3CA0-4C03-BF6A-19FFB352F1CB}" name="Functional Requirement" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{BD144430-D3BE-452E-AC92-0F9CFE819628}" name="Notes" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{690081E5-6AEA-4793-899B-48747C04A283}" name="Priority" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E5783501-62B7-4AE4-8977-DB7FB12502D2}" name="Proposed By" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{CFF24DCB-3CA0-4C03-BF6A-19FFB352F1CB}" name="Functional Requirement" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{BD144430-D3BE-452E-AC92-0F9CFE819628}" name="Notes" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{690081E5-6AEA-4793-899B-48747C04A283}" name="Priority" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{E5783501-62B7-4AE4-8977-DB7FB12502D2}" name="Proposed By" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{45279D79-309C-4BA7-9648-BE6FBE66D3F8}" name="Table245" displayName="Table245" ref="A1:D33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5B8ED29-B2D8-4D32-8727-B863AB9ECDF0}" name="Table242" displayName="Table242" ref="A1:D33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D33" xr:uid="{E3953504-9D1B-481C-AD87-36BE767B8EC0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A890120A-1A50-4689-BC8E-9FDE1A06757B}" name="Functional Requirement" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{904E4E5C-8CCC-4100-B026-B0FB5CC541B8}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FD19AE5F-3061-40CF-B107-224020BAF0F3}" name="Priority" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D00853E1-2C80-4C8E-8BB2-07094E2B0034}" name="Proposed By" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{45279D79-309C-4BA7-9648-BE6FBE66D3F8}" name="Table245" displayName="Table245" ref="A1:D33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:D33" xr:uid="{45279D79-309C-4BA7-9648-BE6FBE66D3F8}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AE1A2A73-2F6A-4FF9-9D53-99647DC63768}" name="Functional Requirement" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F3DE6A2B-3125-4704-9851-2C5297B06E63}" name="Notes" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{DD758B49-4095-4280-90A2-E4A20F9F22A7}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C7DD39F2-B647-49F1-A58C-015CC1093615}" name="Proposed By" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AE1A2A73-2F6A-4FF9-9D53-99647DC63768}" name="Functional Requirement" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{F3DE6A2B-3125-4704-9851-2C5297B06E63}" name="Notes" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{DD758B49-4095-4280-90A2-E4A20F9F22A7}" name="Priority" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{C7DD39F2-B647-49F1-A58C-015CC1093615}" name="Proposed By" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1362,18 +1605,18 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="84.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1401,7 +1644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1415,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1429,7 +1672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1451,7 +1694,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1465,7 +1708,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1479,151 +1722,151 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1638,6 +1881,102 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5F9396-1BEA-4FE5-B9EE-41319F9FB292}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="68.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94BA6DD-BF45-4839-8BE1-EE3A07741D36}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1645,15 +1984,15 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1667,7 +2006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>34</v>
       </c>
@@ -1679,7 +2018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>54</v>
       </c>
@@ -1691,7 +2030,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>58</v>
       </c>
@@ -1703,7 +2042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>59</v>
       </c>
@@ -1715,25 +2054,25 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1744,13 +2083,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5544CA-0854-4CDA-BA28-4F37C7D3A2F2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1761,18 +2102,18 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +2127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1796,7 +2137,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +2147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1816,7 +2157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -1828,7 +2169,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1840,163 +2181,163 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2011,22 +2352,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3958322B-389B-4DEE-85CA-E457D1A9FA6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A68065C-5022-4A16-883E-0431490F0A4A}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2040,207 +2381,199 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2255,22 +2588,292 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3958322B-389B-4DEE-85CA-E457D1A9FA6A}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F308C206-6B02-4764-B49C-1B64148AE93F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2284,7 +2887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -2296,7 +2899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
@@ -2310,31 +2913,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="23"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="24"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>47</v>
       </c>
@@ -2348,23 +2951,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>76</v>
+      </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2377,23 +3002,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B501D21-4606-4980-B9C4-0A99300B81E8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.44140625" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +3032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
@@ -2419,7 +3044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
@@ -2431,7 +3056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
@@ -2439,7 +3064,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>50</v>
       </c>
@@ -2451,7 +3076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>51</v>
       </c>
@@ -2463,132 +3088,31 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1381290C-1C74-4BB7-B6DC-CD17BB0C4795}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2600,22 +3124,155 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1381290C-1C74-4BB7-B6DC-CD17BB0C4795}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3285BAEA-AA6B-4AF4-A9B6-E51B2AF932D8}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +3286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>28</v>
       </c>
@@ -2643,115 +3300,115 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
       <c r="B3" s="26"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="26"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="25"/>
       <c r="B5" s="26"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="26"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="25"/>
       <c r="B7" s="26"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25"/>
       <c r="B8" s="26"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="26"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="26"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="26"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
       <c r="B14" s="26"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="26"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
       <c r="B16" s="26"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
       <c r="B18" s="26"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="26"/>
       <c r="C21" s="25"/>
@@ -2768,23 +3425,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6655AA7F-A4D2-42E3-8D96-EEEE7703AB81}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2798,7 +3455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -2810,7 +3467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>60</v>
       </c>
@@ -2822,37 +3479,51 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2861,100 +3532,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5F9396-1BEA-4FE5-B9EE-41319F9FB292}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="68.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>